<commit_message>
Data too noisy. Reduced for clarity
</commit_message>
<xml_diff>
--- a/Lesson 5/Numerical Diff DataGen.xlsx
+++ b/Lesson 5/Numerical Diff DataGen.xlsx
@@ -396,7 +396,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1694103263471584</v>
+        <v>-0.4131636533673999</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -404,7 +404,7 @@
         <v>0.5</v>
       </c>
       <c r="B3">
-        <v>-0.4773624760855111</v>
+        <v>0.8238509115745072</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0.484236022836257</v>
+        <v>1.400901628879421</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -420,7 +420,7 @@
         <v>1.5</v>
       </c>
       <c r="B5">
-        <v>1.115015587755864</v>
+        <v>2.662840662933722</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>3.806931898631603</v>
+        <v>3.565271434419023</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -436,7 +436,7 @@
         <v>2.5</v>
       </c>
       <c r="B7">
-        <v>3.731007829975275</v>
+        <v>4.390099044047414</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -444,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>5.724158408719827</v>
+        <v>5.084705158429044</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -452,7 +452,7 @@
         <v>3.5</v>
       </c>
       <c r="B9">
-        <v>4.805481026629428</v>
+        <v>6.058480790704488</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -460,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <v>6.036621168603352</v>
+        <v>6.480543120354559</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -468,7 +468,7 @@
         <v>4.5</v>
       </c>
       <c r="B11">
-        <v>7.506430795654722</v>
+        <v>7.744274164899728</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -476,7 +476,7 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>7.656529722095261</v>
+        <v>8.213118453516353</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -484,7 +484,7 @@
         <v>5.5</v>
       </c>
       <c r="B13">
-        <v>8.207891127426857</v>
+        <v>9.771414924822103</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -492,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <v>11.4107544706363</v>
+        <v>11.13288767852672</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -500,7 +500,7 @@
         <v>6.5</v>
       </c>
       <c r="B15">
-        <v>11.42831986655956</v>
+        <v>11.62438237848504</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -508,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>14.57006848856137</v>
+        <v>13.23286338686713</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -516,7 +516,7 @@
         <v>7.5</v>
       </c>
       <c r="B17">
-        <v>12.75292287718321</v>
+        <v>14.2666822772573</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -524,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>14.4427327830585</v>
+        <v>15.35775383255386</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -532,7 +532,7 @@
         <v>8.5</v>
       </c>
       <c r="B19">
-        <v>13.62106680595087</v>
+        <v>16.55257501767783</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>18.30545516947813</v>
+        <v>17.99371871788277</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -548,7 +548,7 @@
         <v>9.5</v>
       </c>
       <c r="B21">
-        <v>20.04668014563882</v>
+        <v>19.31498754323765</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -556,7 +556,7 @@
         <v>10</v>
       </c>
       <c r="B22">
-        <v>20.74675470819404</v>
+        <v>20.10285869029084</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -564,7 +564,7 @@
         <v>10.5</v>
       </c>
       <c r="B23">
-        <v>21.83484950687841</v>
+        <v>21.69747103584839</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -572,7 +572,7 @@
         <v>11</v>
       </c>
       <c r="B24">
-        <v>23.56343498341902</v>
+        <v>23.38256577753764</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -580,7 +580,7 @@
         <v>11.5</v>
       </c>
       <c r="B25">
-        <v>26.31481689551095</v>
+        <v>24.87145510509535</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -588,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <v>24.95575060046218</v>
+        <v>26.6637355542847</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -596,7 +596,7 @@
         <v>12.5</v>
       </c>
       <c r="B27">
-        <v>26.34121461157557</v>
+        <v>27.29120994675154</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <v>28.87889346931867</v>
+        <v>29.46564032812875</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -612,7 +612,7 @@
         <v>13.5</v>
       </c>
       <c r="B29">
-        <v>29.80547078021284</v>
+        <v>31.54783256081483</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -620,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="B30">
-        <v>32.85310734714766</v>
+        <v>32.42340550727129</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -628,7 +628,7 @@
         <v>14.5</v>
       </c>
       <c r="B31">
-        <v>34.69726094946173</v>
+        <v>34.72985608586661</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -636,7 +636,7 @@
         <v>15</v>
       </c>
       <c r="B32">
-        <v>38.11459674350036</v>
+        <v>37.60214223394708</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -644,7 +644,7 @@
         <v>15.5</v>
       </c>
       <c r="B33">
-        <v>38.48087328393576</v>
+        <v>39.71323306898522</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -652,7 +652,7 @@
         <v>16</v>
       </c>
       <c r="B34">
-        <v>40.1294192420863</v>
+        <v>40.9888913641441</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -660,7 +660,7 @@
         <v>16.5</v>
       </c>
       <c r="B35">
-        <v>42.71306224634623</v>
+        <v>43.11569601138837</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -668,7 +668,7 @@
         <v>17</v>
       </c>
       <c r="B36">
-        <v>43.8791410650693</v>
+        <v>45.47121598881147</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -676,7 +676,7 @@
         <v>17.5</v>
       </c>
       <c r="B37">
-        <v>46.61097497265741</v>
+        <v>47.24117131621497</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -684,7 +684,7 @@
         <v>18</v>
       </c>
       <c r="B38">
-        <v>49.95991083298973</v>
+        <v>50.1384477071067</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -692,7 +692,7 @@
         <v>18.5</v>
       </c>
       <c r="B39">
-        <v>53.42006895598967</v>
+        <v>52.36126051287686</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -700,7 +700,7 @@
         <v>19</v>
       </c>
       <c r="B40">
-        <v>56.07624661503669</v>
+        <v>55.03906701522532</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -708,7 +708,7 @@
         <v>19.5</v>
       </c>
       <c r="B41">
-        <v>56.76494544887314</v>
+        <v>58.38839046960703</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -716,7 +716,7 @@
         <v>20</v>
       </c>
       <c r="B42">
-        <v>61.4409286760565</v>
+        <v>60.43854851432661</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -724,7 +724,7 @@
         <v>20.5</v>
       </c>
       <c r="B43">
-        <v>64.6248856762063</v>
+        <v>63.56836076088637</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -732,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="B44">
-        <v>64.69808583731805</v>
+        <v>66.62301075635303</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -740,7 +740,7 @@
         <v>21.5</v>
       </c>
       <c r="B45">
-        <v>69.84646688930597</v>
+        <v>69.43257032278152</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -748,7 +748,7 @@
         <v>22</v>
       </c>
       <c r="B46">
-        <v>73.61921253334684</v>
+        <v>73.26128353070021</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -756,7 +756,7 @@
         <v>22.5</v>
       </c>
       <c r="B47">
-        <v>75.7165566242798</v>
+        <v>76.41689312478887</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -764,7 +764,7 @@
         <v>23</v>
       </c>
       <c r="B48">
-        <v>79.03295099929623</v>
+        <v>79.2507145551281</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -772,7 +772,7 @@
         <v>23.5</v>
       </c>
       <c r="B49">
-        <v>84.12059322176434</v>
+        <v>83.25490107051952</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -780,7 +780,7 @@
         <v>24</v>
       </c>
       <c r="B50">
-        <v>85.81497839032859</v>
+        <v>86.73336770651613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>